<commit_message>
Penyusunan SQL Generator untuk Budget, BudgetSection, dan BudgetLine
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Budgeting.TblBudgetGroup.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Budgeting.TblBudgetGroup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -18,10 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>PERFORM "SchData-OLTP-Budgeting"."Func_TblBudgetGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 108000000000001::bigint, 'CAPEX'::varchar, 'Capital Expenditure'::varchar, '2020-01-01 00:00:00+07'::timestamptz, '9999-12-31 23:59:59+07'::timestamptz);</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>OPEX</t>
   </si>
@@ -33,13 +30,22 @@
   </si>
   <si>
     <t>Capital Expenditure</t>
+  </si>
+  <si>
+    <t>9999-12-31 23:59:59+07</t>
+  </si>
+  <si>
+    <t>2020-01-01 00:00:00+07</t>
+  </si>
+  <si>
+    <t>SYS_PID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,13 +59,32 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,10 +99,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F3"/>
+  <dimension ref="B1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -424,42 +454,70 @@
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="6" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
         <f>TblBudgetType!$B$2</f>
         <v>108000000000001</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="str">
-        <f>CONCATENATE("PERFORM ""SchData-OLTP-Budgeting"".""Func_TblBudgetGroup_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, 108000000000001::bigint, '", C2, "'::varchar, 'Operational Expenditure'::varchar, '2020-01-01 00:00:00+07'::timestamptz, '9999-12-31 23:59:59+07'::timestamptz);")</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>CONCATENATE("PERFORM ""SchData-OLTP-Budgeting"".""Func_TblBudgetGroup_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, ", B2, "::bigint, '", C2, "'::varchar, '", D2, "'::varchar, '", E2, "'::timestamptz, '", F2, "'::timestamptz);")</f>
         <v>PERFORM "SchData-OLTP-Budgeting"."Func_TblBudgetGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 108000000000001::bigint, 'OPEX'::varchar, 'Operational Expenditure'::varchar, '2020-01-01 00:00:00+07'::timestamptz, '9999-12-31 23:59:59+07'::timestamptz);</v>
       </c>
+      <c r="J2" s="5">
+        <v>109000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <f>TblBudgetType!$B$2</f>
         <v>108000000000001</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
+      <c r="H3" s="2" t="str">
+        <f>CONCATENATE("PERFORM ""SchData-OLTP-Budgeting"".""Func_TblBudgetGroup_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, ", B3, "::bigint, '", C3, "'::varchar, '", D3, "'::varchar, '", E3, "'::timestamptz, '", F3, "'::timestamptz);")</f>
+        <v>PERFORM "SchData-OLTP-Budgeting"."Func_TblBudgetGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 108000000000001::bigint, 'CAPEX'::varchar, 'Capital Expenditure'::varchar, '2020-01-01 00:00:00+07'::timestamptz, '9999-12-31 23:59:59+07'::timestamptz);</v>
+      </c>
+      <c r="J3" s="5">
+        <v>109000000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>